<commit_message>
fix dijkstra some more stats and workspace
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>one run more than 1 min long</t>
   </si>
@@ -38,13 +38,19 @@
     <t>moves</t>
   </si>
   <si>
-    <t>D moves</t>
-  </si>
-  <si>
     <t>in 4.15s</t>
   </si>
   <si>
     <t>bfs</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>bfs test</t>
+  </si>
+  <si>
+    <t>côté</t>
   </si>
 </sst>
 </file>
@@ -178,11 +184,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>time (s)</c:v>
+                  <c:v>moves</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -226,69 +232,43 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>scale</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.1</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6</c:v>
+                  <c:v>16.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.05</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.35</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>21.45</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.4</c:v>
+                  <c:v>88.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -296,7 +276,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8989-473A-9008-BF0B4B9C8D98}"/>
+              <c16:uniqueId val="{00000001-B78A-4C7F-89A7-A4EC7207AE64}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -397,8 +377,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -467,7 +448,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>time in seconds</a:t>
+                  <a:t>moves</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1036,6 +1017,515 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>test du BFS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>moves</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$32:$E$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$32:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9530-493F-8337-6A964800FC1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1180817120"/>
+        <c:axId val="1180809216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1180817120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>côté</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> du labyrinthe carré</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1180809216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1180809216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>mouvements du rat</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1180817120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1116,6 +1606,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -2177,6 +2707,544 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -2246,6 +3314,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2517,10 +3615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2533,10 +3631,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2548,10 +3646,10 @@
         <v>3.1</v>
       </c>
       <c r="C2">
-        <v>3.5</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>2.1</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2562,6 +3660,12 @@
         <f>72/20</f>
         <v>3.6</v>
       </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>16.399999999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -2571,6 +3675,12 @@
         <f>101/20</f>
         <v>5.05</v>
       </c>
+      <c r="C4">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -2580,6 +3690,12 @@
         <f>127/20</f>
         <v>6.35</v>
       </c>
+      <c r="C5">
+        <v>81</v>
+      </c>
+      <c r="D5">
+        <v>88.7</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -2598,21 +3714,18 @@
         <f>429/20</f>
         <v>21.45</v>
       </c>
-      <c r="D7">
-        <v>11.1</v>
-      </c>
       <c r="E7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -2671,7 +3784,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2679,7 +3792,7 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2687,7 +3800,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -2695,7 +3808,7 @@
         <v>30.8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>21</v>
       </c>
@@ -2703,7 +3816,7 @@
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>23</v>
       </c>
@@ -2711,7 +3824,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>25</v>
       </c>
@@ -2719,7 +3832,7 @@
         <v>43.3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>27</v>
       </c>
@@ -2727,7 +3840,7 @@
         <v>49.8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>29</v>
       </c>
@@ -2735,7 +3848,7 @@
         <v>51.4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>31</v>
       </c>
@@ -2743,7 +3856,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>33</v>
       </c>
@@ -2751,7 +3864,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>35</v>
       </c>
@@ -2759,7 +3872,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>37</v>
       </c>
@@ -2767,7 +3880,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>39</v>
       </c>
@@ -2775,52 +3888,161 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>41</v>
       </c>
       <c r="B30">
         <v>83.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>43</v>
       </c>
       <c r="B31">
         <v>85.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>45</v>
       </c>
       <c r="B32">
         <v>80.7</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <f>E32-1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>47</v>
       </c>
       <c r="B33">
         <v>85.4</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ref="F33:F43" si="0">E33-1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>49</v>
       </c>
       <c r="B34">
         <v>97.1</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>51</v>
       </c>
       <c r="B35">
         <v>94</v>
+      </c>
+      <c r="E35">
+        <v>9</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>11</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>13</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>15</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>17</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>19</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>21</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>23</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>25</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduces parameters, created exaustive search
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poltg\Documents\imtcode\Pyrat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E7B51C-E99C-4321-82F1-EFE8F02AB143}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B707726-02CA-4CD5-8493-5CC201B11825}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15645" yWindow="4200" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>one run more than 1 min long</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>dfs</t>
+  </si>
+  <si>
+    <t>ants</t>
+  </si>
+  <si>
+    <t>greed</t>
+  </si>
+  <si>
+    <t>bruteforce</t>
+  </si>
+  <si>
+    <t>BnB</t>
   </si>
 </sst>
 </file>
@@ -1706,6 +1718,465 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Time of execution</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bruteforce</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$L$31:$L$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$31:$M$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.37E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D17B-472C-8830-E4C471B4BE3C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BnB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$L$31:$L$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$31:$N$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.47E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7399999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D17B-472C-8830-E4C471B4BE3C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="912202496"/>
+        <c:axId val="810493680"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="912202496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="810493680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="810493680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="912202496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1826,6 +2297,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -3437,20 +3948,516 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
+      <xdr:colOff>325755</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3542,6 +4549,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25D8B9C8-9644-4601-916D-9522ACCC4124}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3813,13 +4856,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="T45" sqref="T45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3982,7 +5028,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3990,7 +5036,7 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3998,7 +5044,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -4006,7 +5052,7 @@
         <v>30.8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -4014,7 +5060,7 @@
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>23</v>
       </c>
@@ -4022,7 +5068,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>25</v>
       </c>
@@ -4030,7 +5076,7 @@
         <v>43.3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>27</v>
       </c>
@@ -4038,7 +5084,7 @@
         <v>49.8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>29</v>
       </c>
@@ -4046,7 +5092,7 @@
         <v>51.4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>31</v>
       </c>
@@ -4054,7 +5100,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>33</v>
       </c>
@@ -4062,7 +5108,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>35</v>
       </c>
@@ -4070,7 +5116,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>37</v>
       </c>
@@ -4078,7 +5124,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>39</v>
       </c>
@@ -4086,7 +5132,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>41</v>
       </c>
@@ -4099,8 +5145,20 @@
       <c r="G30" t="s">
         <v>9</v>
       </c>
+      <c r="I30" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>43</v>
       </c>
@@ -4116,8 +5174,23 @@
       <c r="G31" t="s">
         <v>9</v>
       </c>
+      <c r="I31">
+        <v>419</v>
+      </c>
+      <c r="J31">
+        <v>490</v>
+      </c>
+      <c r="L31">
+        <v>5</v>
+      </c>
+      <c r="M31">
+        <v>1.37E-2</v>
+      </c>
+      <c r="N31">
+        <v>1.47E-2</v>
+      </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>45</v>
       </c>
@@ -4134,8 +5207,23 @@
       <c r="G32">
         <v>3</v>
       </c>
+      <c r="I32">
+        <v>437</v>
+      </c>
+      <c r="J32">
+        <v>474</v>
+      </c>
+      <c r="L32">
+        <v>7</v>
+      </c>
+      <c r="M32">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="N32">
+        <v>4.7399999999999998E-2</v>
+      </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>47</v>
       </c>
@@ -4152,8 +5240,23 @@
       <c r="G33">
         <v>8</v>
       </c>
+      <c r="I33">
+        <v>393</v>
+      </c>
+      <c r="J33">
+        <v>438</v>
+      </c>
+      <c r="L33">
+        <v>9</v>
+      </c>
+      <c r="M33">
+        <v>1.92</v>
+      </c>
+      <c r="N33">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>49</v>
       </c>
@@ -4170,8 +5273,23 @@
       <c r="G34">
         <v>12</v>
       </c>
+      <c r="I34">
+        <v>374</v>
+      </c>
+      <c r="J34">
+        <v>391</v>
+      </c>
+      <c r="L34">
+        <v>10</v>
+      </c>
+      <c r="M34">
+        <v>21.7</v>
+      </c>
+      <c r="N34">
+        <v>2.31</v>
+      </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>51</v>
       </c>
@@ -4188,8 +5306,14 @@
       <c r="G35">
         <v>16</v>
       </c>
+      <c r="I35">
+        <v>557</v>
+      </c>
+      <c r="J35">
+        <v>629</v>
+      </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E36">
         <v>11</v>
       </c>
@@ -4200,8 +5324,14 @@
       <c r="G36">
         <v>20</v>
       </c>
+      <c r="I36">
+        <v>470</v>
+      </c>
+      <c r="J36">
+        <v>521</v>
+      </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>13</v>
       </c>
@@ -4212,8 +5342,14 @@
       <c r="G37">
         <v>24</v>
       </c>
+      <c r="I37">
+        <v>489</v>
+      </c>
+      <c r="J37">
+        <v>493</v>
+      </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E38">
         <v>15</v>
       </c>
@@ -4224,8 +5360,14 @@
       <c r="G38">
         <v>28</v>
       </c>
+      <c r="I38">
+        <v>267</v>
+      </c>
+      <c r="J38">
+        <v>299</v>
+      </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E39">
         <v>17</v>
       </c>
@@ -4236,8 +5378,14 @@
       <c r="G39">
         <v>32</v>
       </c>
+      <c r="I39">
+        <v>373</v>
+      </c>
+      <c r="J39">
+        <v>463</v>
+      </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>19</v>
       </c>
@@ -4248,8 +5396,14 @@
       <c r="G40">
         <v>36</v>
       </c>
+      <c r="I40">
+        <v>369</v>
+      </c>
+      <c r="J40">
+        <v>383</v>
+      </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E41">
         <v>21</v>
       </c>
@@ -4260,8 +5414,14 @@
       <c r="G41">
         <v>40</v>
       </c>
+      <c r="I41">
+        <v>318</v>
+      </c>
+      <c r="J41">
+        <v>334</v>
+      </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E42">
         <v>23</v>
       </c>
@@ -4272,8 +5432,14 @@
       <c r="G42">
         <v>44</v>
       </c>
+      <c r="I42">
+        <v>425</v>
+      </c>
+      <c r="J42">
+        <v>473</v>
+      </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E43">
         <v>25</v>
       </c>
@@ -4283,6 +5449,84 @@
       </c>
       <c r="G43">
         <v>48</v>
+      </c>
+      <c r="I43">
+        <v>460</v>
+      </c>
+      <c r="J43">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>384</v>
+      </c>
+      <c r="J44">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>394</v>
+      </c>
+      <c r="J45">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>243</v>
+      </c>
+      <c r="J46">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>349</v>
+      </c>
+      <c r="J47">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>433</v>
+      </c>
+      <c r="J48">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>428</v>
+      </c>
+      <c r="J49">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="50" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>463</v>
+      </c>
+      <c r="J50">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="51" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>378</v>
+      </c>
+      <c r="J51">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="52" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>460</v>
+      </c>
+      <c r="J52">
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>